<commit_message>
Diseño de la hoja excel Backlog
</commit_message>
<xml_diff>
--- a/Analisis/US-Sprint.xlsx
+++ b/Analisis/US-Sprint.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +315,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -378,12 +386,232 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="double">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="double">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="double">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -393,171 +621,21 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="double">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="double">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top style="double">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="double">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="double">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="double">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="double">
-        <color indexed="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -568,23 +646,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -599,18 +677,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,7 +987,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -891,229 +995,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="A2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="45" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="46" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="C4" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="46" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="A5" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="46" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="42"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="46" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="42"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="C7" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="46" t="s">
         <v>21</v>
       </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="42"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="A8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="46" t="s">
         <v>27</v>
       </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="42"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="C9" t="s">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="46" t="s">
         <v>28</v>
       </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="A10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="46" t="s">
         <v>33</v>
       </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="42"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="C11" t="s">
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="46" t="s">
         <v>38</v>
       </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="C12" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="46" t="s">
         <v>34</v>
       </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="46"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="46" t="s">
         <v>35</v>
       </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" t="s">
+      <c r="A14" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="46" t="s">
         <v>42</v>
       </c>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="C15" t="s">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="46" t="s">
         <v>43</v>
       </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="42"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" t="s">
+      <c r="A16" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17" t="s">
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="42"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="46" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" t="s">
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="42"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="47" t="s">
         <v>48</v>
       </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="G23" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1134,13 +1367,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -1149,7 +1382,7 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3" t="s">
@@ -1158,7 +1391,7 @@
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="39"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -1167,7 +1400,7 @@
       <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -1176,7 +1409,7 @@
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -1185,16 +1418,16 @@
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1203,7 +1436,7 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -1230,7 +1463,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1267,15 +1500,15 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1312,10 +1545,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1344,641 +1577,641 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" thickBot="1">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="N2" s="14"/>
+      <c r="C2" s="8"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="12">
         <v>2</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="12">
         <v>4</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="12">
         <v>5</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="12">
         <v>6</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="12">
         <v>7</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="12">
         <v>8</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="12">
         <v>9</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="48" customHeight="1" thickBot="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="40" t="str">
+      <c r="C4" s="35" t="str">
         <f>T(B5)</f>
         <v>Administrar datos generales de los clientes.</v>
       </c>
-      <c r="D4" s="40" t="str">
+      <c r="D4" s="35" t="str">
         <f>T(B6)</f>
         <v>Administrar cartelera de peliculas.</v>
       </c>
-      <c r="E4" s="40" t="str">
+      <c r="E4" s="35" t="str">
         <f>T(B7)</f>
         <v>Crear buscador de peliculas</v>
       </c>
-      <c r="F4" s="40" t="str">
+      <c r="F4" s="35" t="str">
         <f>T(B8)</f>
         <v>Implementar carrito de compras.</v>
       </c>
-      <c r="G4" s="40" t="str">
+      <c r="G4" s="35" t="str">
         <f>T(B9)</f>
         <v>Administrar ventas.</v>
       </c>
-      <c r="H4" s="40" t="str">
+      <c r="H4" s="35" t="str">
         <f>T(B10)</f>
         <v>Notificacion de clientes.</v>
       </c>
-      <c r="I4" s="41" t="str">
+      <c r="I4" s="36" t="str">
         <f>T(B11)</f>
         <v/>
       </c>
-      <c r="J4" s="41" t="str">
+      <c r="J4" s="36" t="str">
         <f>T(B12)</f>
         <v/>
       </c>
-      <c r="K4" s="40" t="str">
+      <c r="K4" s="35" t="str">
         <f>T(B13)</f>
         <v/>
       </c>
-      <c r="L4" s="42" t="str">
+      <c r="L4" s="37" t="str">
         <f>T(B14)</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:14" ht="48" customHeight="1" thickBot="1">
-      <c r="A5" s="19">
+      <c r="A5" s="14">
         <v>1</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <v>5</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="17">
         <v>2</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="17">
         <v>5</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="17">
         <v>5</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="17">
         <v>2</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="23"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:14" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A6" s="19">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="19">
         <f>IF(D5="","",1/D5)</f>
         <v>0.2</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <v>1</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="17">
         <v>5</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="17">
         <v>8</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="17">
         <v>8</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="17">
         <v>2</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="23"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="36" customHeight="1" thickBot="1">
-      <c r="A7" s="19">
+      <c r="A7" s="14">
         <v>3</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="19">
         <f>IF(E5="","",1/E5)</f>
         <v>0.5</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="19">
         <f>IF(E6="","",1/E6)</f>
         <v>0.2</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="16">
         <v>1</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="17">
         <v>8</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="17">
         <v>8</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="17">
         <v>2</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="23"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:14" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A8" s="19">
+      <c r="A8" s="14">
         <v>4</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="19">
         <f>IF(F5="","",1/F5)</f>
         <v>0.2</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="19">
         <f>IF(F6="","",1/F6)</f>
         <v>0.125</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="19">
         <f>IF(F7="","",1/F7)</f>
         <v>0.125</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="16">
         <v>1</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="17">
         <v>5</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="17">
         <v>2</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="23"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="19">
+      <c r="A9" s="14">
         <v>5</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="19">
         <f>IF(G5="","",1/G5)</f>
         <v>0.2</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="19">
         <f>IF(G6="","",1/G6)</f>
         <v>0.125</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="19">
         <f>IF(G7="","",1/G7)</f>
         <v>0.125</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="19">
         <f>IF(G8="","",1/G8)</f>
         <v>0.2</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="16">
         <v>1</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="17">
         <v>2</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="23"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:14" ht="30.75" thickBot="1">
-      <c r="A10" s="19">
+      <c r="A10" s="14">
         <v>6</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="19">
         <f>IF(H5="","",1/G6)</f>
         <v>0.125</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="19">
         <f>IF(H6="","",1/H6)</f>
         <v>0.5</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="19">
         <f>IF(H7="","",1/H7)</f>
         <v>0.5</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="19">
         <f>IF(H8="","",1/H8)</f>
         <v>0.5</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="19">
         <f>IF(H9="","",1/H9)</f>
         <v>0.5</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="16">
         <v>1</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="23"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A11" s="19">
+      <c r="A11" s="14">
         <v>7</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="24" t="str">
+      <c r="B11" s="38"/>
+      <c r="C11" s="19" t="str">
         <f>IF(I5="","",1/G7)</f>
         <v/>
       </c>
-      <c r="D11" s="24" t="str">
+      <c r="D11" s="19" t="str">
         <f>IF(I6="","",1/I6)</f>
         <v/>
       </c>
-      <c r="E11" s="24" t="str">
+      <c r="E11" s="19" t="str">
         <f>IF(I7="","",1/I7)</f>
         <v/>
       </c>
-      <c r="F11" s="24" t="str">
+      <c r="F11" s="19" t="str">
         <f>IF(I8="","",1/I8)</f>
         <v/>
       </c>
-      <c r="G11" s="24" t="str">
+      <c r="G11" s="19" t="str">
         <f>IF(I9="","",1/I9)</f>
         <v/>
       </c>
-      <c r="H11" s="24" t="str">
+      <c r="H11" s="19" t="str">
         <f>IF(I10="","",1/I10)</f>
         <v/>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="16">
         <v>1</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A12" s="19">
+      <c r="A12" s="14">
         <v>8</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="24" t="str">
+      <c r="B12" s="38"/>
+      <c r="C12" s="19" t="str">
         <f>IF(J5="","",1/G8)</f>
         <v/>
       </c>
-      <c r="D12" s="24" t="str">
+      <c r="D12" s="19" t="str">
         <f>IF(J6="","",1/J6)</f>
         <v/>
       </c>
-      <c r="E12" s="24" t="str">
+      <c r="E12" s="19" t="str">
         <f>IF(J7="","",1/J7)</f>
         <v/>
       </c>
-      <c r="F12" s="24" t="str">
+      <c r="F12" s="19" t="str">
         <f>IF(J8="","",1/J8)</f>
         <v/>
       </c>
-      <c r="G12" s="24" t="str">
+      <c r="G12" s="19" t="str">
         <f>IF(J9="","",1/J9)</f>
         <v/>
       </c>
-      <c r="H12" s="24" t="str">
+      <c r="H12" s="19" t="str">
         <f>IF(J10="","",1/J10)</f>
         <v/>
       </c>
-      <c r="I12" s="24" t="str">
+      <c r="I12" s="19" t="str">
         <f>IF(J11="","",1/J11)</f>
         <v/>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="16">
         <v>1</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A13" s="19">
+      <c r="A13" s="14">
         <v>9</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="24" t="str">
+      <c r="B13" s="38"/>
+      <c r="C13" s="19" t="str">
         <f>IF(K5="","",1/G9)</f>
         <v/>
       </c>
-      <c r="D13" s="24" t="str">
+      <c r="D13" s="19" t="str">
         <f>IF(K6="","",1/K6)</f>
         <v/>
       </c>
-      <c r="E13" s="24" t="str">
+      <c r="E13" s="19" t="str">
         <f>IF(K7="","",1/K7)</f>
         <v/>
       </c>
-      <c r="F13" s="24" t="str">
+      <c r="F13" s="19" t="str">
         <f>IF(K8="","",1/K8)</f>
         <v/>
       </c>
-      <c r="G13" s="24" t="str">
+      <c r="G13" s="19" t="str">
         <f>IF(K9="","",1/K9)</f>
         <v/>
       </c>
-      <c r="H13" s="24" t="str">
+      <c r="H13" s="19" t="str">
         <f>IF(K10="","",1/K10)</f>
         <v/>
       </c>
-      <c r="I13" s="24" t="str">
+      <c r="I13" s="19" t="str">
         <f>IF(K11="","",1/K11)</f>
         <v/>
       </c>
-      <c r="J13" s="24" t="str">
+      <c r="J13" s="19" t="str">
         <f>IF(K12="","",1/K12)</f>
         <v/>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="16">
         <v>1</v>
       </c>
-      <c r="L13" s="23"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="19">
+      <c r="A14" s="14">
         <v>10</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="str">
+      <c r="B14" s="20"/>
+      <c r="C14" s="19" t="str">
         <f>IF(L5="","",1/G10)</f>
         <v/>
       </c>
-      <c r="D14" s="24" t="str">
+      <c r="D14" s="19" t="str">
         <f>IF(L6="","",1/L6)</f>
         <v/>
       </c>
-      <c r="E14" s="24" t="str">
+      <c r="E14" s="19" t="str">
         <f>IF(L7="","",1/L7)</f>
         <v/>
       </c>
-      <c r="F14" s="24" t="str">
+      <c r="F14" s="19" t="str">
         <f>IF(L8="","",1/L8)</f>
         <v/>
       </c>
-      <c r="G14" s="24" t="str">
+      <c r="G14" s="19" t="str">
         <f>IF(L9="","",1/L9)</f>
         <v/>
       </c>
-      <c r="H14" s="24" t="str">
+      <c r="H14" s="19" t="str">
         <f>IF(L10="","",1/L10)</f>
         <v/>
       </c>
-      <c r="I14" s="24" t="str">
+      <c r="I14" s="19" t="str">
         <f>IF(L11="","",1/L11)</f>
         <v/>
       </c>
-      <c r="J14" s="24" t="str">
+      <c r="J14" s="19" t="str">
         <f>IF(L12="","",1/L12)</f>
         <v/>
       </c>
-      <c r="K14" s="24" t="str">
+      <c r="K14" s="19" t="str">
         <f>IF(L13="","",1/L13)</f>
         <v/>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="19">
         <f>IF(C6="","",SUM(C5:C14))</f>
         <v>2.2250000000000001</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="19">
         <f t="shared" ref="D15:L15" si="0">IF(D5="","",SUM(D5:D14))</f>
         <v>6.95</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="19">
         <f t="shared" si="0"/>
         <v>8.75</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>22.7</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="19">
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="I15" s="24" t="str">
+      <c r="I15" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J15" s="24" t="str">
+      <c r="J15" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K15" s="24" t="str">
+      <c r="K15" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L15" s="28" t="str">
+      <c r="L15" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="31"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickTop="1"/>
     <row r="18" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A20" s="19">
+      <c r="A20" s="14">
         <v>1</v>
       </c>
-      <c r="B20" s="43" t="str">
+      <c r="B20" s="38" t="str">
         <f t="shared" ref="B20:B25" si="1">B5</f>
         <v>Administrar datos generales de los clientes.</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="19">
         <f>G15</f>
         <v>27.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45.75" thickBot="1">
-      <c r="A21" s="19">
+      <c r="A21" s="14">
         <v>2</v>
       </c>
-      <c r="B21" s="43" t="str">
+      <c r="B21" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Administrar cartelera de peliculas.</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="19">
         <f>F15</f>
         <v>22.7</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30.75" thickBot="1">
-      <c r="A22" s="19">
+      <c r="A22" s="14">
         <v>3</v>
       </c>
-      <c r="B22" s="43" t="str">
+      <c r="B22" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Crear buscador de peliculas</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="19">
         <f>H15</f>
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45.75" thickBot="1">
-      <c r="A23" s="19">
+      <c r="A23" s="14">
         <v>4</v>
       </c>
-      <c r="B23" s="43" t="str">
+      <c r="B23" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Implementar carrito de compras.</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="19">
         <f>E15</f>
         <v>8.75</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30.75" thickBot="1">
-      <c r="A24" s="19">
+      <c r="A24" s="14">
         <v>5</v>
       </c>
-      <c r="B24" s="43" t="str">
+      <c r="B24" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Administrar ventas.</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="19">
         <f>D15</f>
         <v>6.95</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30.75" thickBot="1">
-      <c r="A25" s="19">
+      <c r="A25" s="14">
         <v>6</v>
       </c>
-      <c r="B25" s="43" t="str">
+      <c r="B25" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Notificacion de clientes.</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="19">
         <f>C15</f>
         <v>2.2250000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
     </row>
     <row r="44" spans="3:14">
-      <c r="C44" s="32"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="3:14">
-      <c r="M45" s="33"/>
-      <c r="N45" s="34"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="29"/>
     </row>
     <row r="46" spans="3:14">
-      <c r="N46" s="34"/>
+      <c r="N46" s="29"/>
     </row>
     <row r="47" spans="3:14">
-      <c r="G47" s="35"/>
-      <c r="H47" s="37"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="36"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="32"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="31"/>
     </row>
     <row r="48" spans="3:14">
-      <c r="G48" s="35"/>
-      <c r="H48" s="37"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="32"/>
     </row>
     <row r="50" spans="2:3">
-      <c r="B50" s="38"/>
+      <c r="B50" s="33"/>
     </row>
     <row r="54" spans="2:3">
-      <c r="C54" s="32"/>
+      <c r="C54" s="27"/>
     </row>
   </sheetData>
   <sortState ref="B19:C26">
@@ -1992,61 +2225,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75.75" thickBot="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="60.75" thickBot="1">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="45.75" thickBot="1">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arquitectura del proyecto en IDE Netbeans 7.4
</commit_message>
<xml_diff>
--- a/Analisis/US-Sprint.xlsx
+++ b/Analisis/US-Sprint.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPC\Evolucion\Trabajo\Analisis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="Matriz" sheetId="4" r:id="rId3"/>
     <sheet name="Sprints" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -231,12 +236,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -987,21 +992,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
@@ -1013,7 +1018,7 @@
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1070,7 @@
       <c r="I2" s="45"/>
       <c r="J2" s="42"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="46"/>
       <c r="C3" s="51" t="s">
@@ -1081,7 +1086,7 @@
       <c r="I3" s="46"/>
       <c r="J3" s="42"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="46"/>
       <c r="C4" s="46" t="s">
@@ -1097,7 +1102,7 @@
       <c r="I4" s="46"/>
       <c r="J4" s="42"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>16</v>
       </c>
@@ -1117,7 +1122,7 @@
       <c r="I5" s="46"/>
       <c r="J5" s="42"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="46"/>
       <c r="B6" s="46"/>
       <c r="C6" s="51" t="s">
@@ -1133,7 +1138,7 @@
       <c r="I6" s="46"/>
       <c r="J6" s="42"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46" t="s">
@@ -1149,7 +1154,7 @@
       <c r="I7" s="46"/>
       <c r="J7" s="42"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>24</v>
       </c>
@@ -1169,7 +1174,7 @@
       <c r="I8" s="46"/>
       <c r="J8" s="42"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46" t="s">
@@ -1185,7 +1190,7 @@
       <c r="I9" s="46"/>
       <c r="J9" s="42"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>30</v>
       </c>
@@ -1205,7 +1210,7 @@
       <c r="I10" s="46"/>
       <c r="J10" s="42"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="46"/>
       <c r="C11" s="46" t="s">
@@ -1221,7 +1226,7 @@
       <c r="I11" s="46"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="46"/>
       <c r="C12" s="46" t="s">
@@ -1237,7 +1242,7 @@
       <c r="I12" s="46"/>
       <c r="J12" s="42"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="46"/>
       <c r="C13" s="51" t="s">
@@ -1253,7 +1258,7 @@
       <c r="I13" s="46"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
         <v>40</v>
       </c>
@@ -1273,7 +1278,7 @@
       <c r="I14" s="46"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
       <c r="B15" s="46"/>
       <c r="C15" s="46" t="s">
@@ -1289,7 +1294,7 @@
       <c r="I15" s="46"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>44</v>
       </c>
@@ -1309,7 +1314,7 @@
       <c r="I16" s="46"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
       <c r="B17" s="46"/>
       <c r="C17" s="46" t="s">
@@ -1325,7 +1330,7 @@
       <c r="I17" s="46"/>
       <c r="J17" s="42"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47" t="s">
@@ -1341,7 +1346,7 @@
       <c r="I18" s="47"/>
       <c r="J18" s="43"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23" s="54"/>
     </row>
   </sheetData>
@@ -1351,14 +1356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
@@ -1366,7 +1371,7 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1380,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1384,7 +1389,7 @@
       </c>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1393,7 +1398,7 @@
       </c>
       <c r="F3" s="34"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1402,7 +1407,7 @@
       </c>
       <c r="F4" s="34"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1411,7 +1416,7 @@
       </c>
       <c r="F5" s="34"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1420,7 +1425,7 @@
       </c>
       <c r="F6" s="34"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
@@ -1429,7 +1434,7 @@
       </c>
       <c r="F7" s="34"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1438,7 +1443,7 @@
       </c>
       <c r="F8" s="34"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1446,7 +1451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1454,7 +1459,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1462,12 +1467,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1475,7 +1480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1483,7 +1488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1491,7 +1496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1499,12 +1504,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1512,7 +1517,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1520,7 +1525,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1528,7 +1533,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1541,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1544,7 +1549,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75">
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -1559,14 +1564,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
@@ -1576,7 +1581,7 @@
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
@@ -1586,14 +1591,14 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75" thickBot="1">
+    <row r="2" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="8"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>63</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="48" customHeight="1" thickBot="1">
+    <row r="4" spans="1:14" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>64</v>
@@ -1677,7 +1682,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="48" customHeight="1" thickBot="1">
+    <row r="5" spans="1:14" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>1</v>
       </c>
@@ -1707,7 +1712,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:14" ht="41.25" customHeight="1" thickBot="1">
+    <row r="6" spans="1:14" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>2</v>
       </c>
@@ -1738,7 +1743,7 @@
       <c r="K6" s="17"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:14" ht="36" customHeight="1" thickBot="1">
+    <row r="7" spans="1:14" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>3</v>
       </c>
@@ -1770,7 +1775,7 @@
       <c r="K7" s="17"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="1:14" ht="43.5" customHeight="1" thickBot="1">
+    <row r="8" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>4</v>
       </c>
@@ -1803,7 +1808,7 @@
       <c r="K8" s="17"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1">
+    <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>5</v>
       </c>
@@ -1837,7 +1842,7 @@
       <c r="K9" s="17"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:14" ht="30.75" thickBot="1">
+    <row r="10" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>6</v>
       </c>
@@ -1872,7 +1877,7 @@
       <c r="K10" s="17"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>7</v>
       </c>
@@ -1908,7 +1913,7 @@
       <c r="K11" s="17"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>8</v>
       </c>
@@ -1947,7 +1952,7 @@
       <c r="K12" s="17"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>9</v>
       </c>
@@ -1989,7 +1994,7 @@
       </c>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>10</v>
       </c>
@@ -2034,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
         <v>65</v>
@@ -2080,7 +2085,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -2094,9 +2099,9 @@
       <c r="K16" s="25"/>
       <c r="L16" s="26"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickTop="1"/>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="38" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2109,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>1</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45.75" thickBot="1">
+    <row r="21" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>2</v>
       </c>
@@ -2130,7 +2135,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30.75" thickBot="1">
+    <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>3</v>
       </c>
@@ -2143,7 +2148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45.75" thickBot="1">
+    <row r="23" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>4</v>
       </c>
@@ -2156,7 +2161,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30.75" thickBot="1">
+    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>5</v>
       </c>
@@ -2169,7 +2174,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30.75" thickBot="1">
+    <row r="25" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>6</v>
       </c>
@@ -2182,35 +2187,35 @@
         <v>2.2250000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
     </row>
-    <row r="44" spans="3:14">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C44" s="27"/>
     </row>
-    <row r="45" spans="3:14">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="M45" s="28"/>
       <c r="N45" s="29"/>
     </row>
-    <row r="46" spans="3:14">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N46" s="29"/>
     </row>
-    <row r="47" spans="3:14">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G47" s="30"/>
       <c r="H47" s="32"/>
       <c r="M47" s="30"/>
       <c r="N47" s="31"/>
     </row>
-    <row r="48" spans="3:14">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G48" s="30"/>
       <c r="H48" s="32"/>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="33"/>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C54" s="27"/>
     </row>
   </sheetData>
@@ -2222,16 +2227,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
@@ -2245,37 +2250,37 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75.75" thickBot="1">
+    <row r="2" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="40"/>
     </row>
-    <row r="3" spans="1:4" ht="60.75" thickBot="1">
+    <row r="3" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="60.75" thickBot="1">
+    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:4" ht="60.75" thickBot="1">
+    <row r="5" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="40"/>
     </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1">
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="40"/>
     </row>
-    <row r="7" spans="1:4" ht="45.75" thickBot="1">
+    <row r="7" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Se agregan las paginas y dependencia del proyecto core
</commit_message>
<xml_diff>
--- a/Analisis/US-Sprint.xlsx
+++ b/Analisis/US-Sprint.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Sprint 1</t>
   </si>
   <si>
-    <t>Permite a usuario comprar entrada.</t>
-  </si>
-  <si>
     <t>Sprint 2</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Resultado</t>
+  </si>
+  <si>
+    <t>Administracion de usuarios y peliculas</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,170 +1391,179 @@
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F3" s="34"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F6" s="34"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="34"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="34"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1567,7 +1576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1593,17 +1602,17 @@
     </row>
     <row r="2" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
@@ -1639,7 +1648,7 @@
     <row r="4" spans="1:14" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="35" t="str">
         <f>T(B5)</f>
@@ -2042,7 +2051,7 @@
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="19">
         <f>IF(C6="","",SUM(C5:C14))</f>
@@ -2106,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2231,7 +2240,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,10 +2253,10 @@
         <v>55</v>
       </c>
       <c r="C1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="38" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,7 +2269,7 @@
       <c r="A3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="B3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
@@ -2284,9 +2293,10 @@
       <c r="A7" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>